<commit_message>
Git command - add line 28
</commit_message>
<xml_diff>
--- a/Git command.xlsx
+++ b/Git command.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Doucument\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Lệnh</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>di chuyển Head về sau các phiên bản, 1 câu lệnh tương ứng với di chuyển về sau 1 phiên bản lệnh commit</t>
+  </si>
+  <si>
+    <t>everything</t>
   </si>
 </sst>
 </file>
@@ -502,32 +505,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -536,6 +533,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,18 +867,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
@@ -914,27 +917,27 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="27" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -946,7 +949,7 @@
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -956,7 +959,7 @@
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
@@ -966,39 +969,39 @@
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1010,43 +1013,43 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="16" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="5"/>
@@ -1076,23 +1079,23 @@
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="14" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="5"/>
@@ -1104,7 +1107,7 @@
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
@@ -1114,7 +1117,7 @@
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
@@ -1122,10 +1125,15 @@
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="5"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Git command - add line 29
</commit_message>
<xml_diff>
--- a/Git command.xlsx
+++ b/Git command.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Lệnh</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>everything</t>
+  </si>
+  <si>
+    <t>fine</t>
   </si>
 </sst>
 </file>
@@ -854,7 +857,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
@@ -1133,6 +1136,11 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Git command - delete line 29
</commit_message>
<xml_diff>
--- a/Git command.xlsx
+++ b/Git command.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Lệnh</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>everything</t>
-  </si>
-  <si>
-    <t>fine</t>
   </si>
 </sst>
 </file>
@@ -857,7 +854,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
@@ -1136,11 +1133,6 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>